<commit_message>
completed download combined table in excel
</commit_message>
<xml_diff>
--- a/aml/combined_flt3_results.xlsx
+++ b/aml/combined_flt3_results.xlsx
@@ -96,7 +96,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -403,100 +404,103 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="5" width="15.7109375" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>243</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>0.04</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>243</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>0.037</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2"/>
-      <c r="B3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="1">
         <v>207</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>0.34</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>207</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>0.284</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="2"/>
-      <c r="B4" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>98</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>0.008999999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>201</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>1.39</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>201</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>0.609</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="2"/>
-      <c r="B6" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>13</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>0.008</v>
       </c>
     </row>

</xml_diff>